<commit_message>
Competition Task Excel data reader third commit
</commit_message>
<xml_diff>
--- a/DataReader/MARS Project.xlsx
+++ b/DataReader/MARS Project.xlsx
@@ -12,9 +12,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Sub Category</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Skill Exchangev Tags</t>
+  </si>
   <si>
     <t>Test Analyst</t>
+  </si>
+  <si>
+    <t>I can analyze your system and can give you the best IT solution</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>Designing</t>
   </si>
 </sst>
 </file>
@@ -22,8 +55,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
@@ -50,6 +88,9 @@
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -60,18 +101,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A2"/>
+  <sheetPr>
+    <tabColor rgb="FF000000"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.335222244262695" customWidth="1"/>
+    <col min="1" max="1" width="10.013422012329102" customWidth="1"/>
+    <col min="2" max="2" width="55.552101135253906" customWidth="1"/>
+    <col min="3" max="3" width="19.216917037963867" customWidth="1"/>
+    <col min="4" max="4" width="12.537323951721191" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.796436309814453" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="20" customHeight="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>